<commit_message>
EUR first pass: fixed RelinkableHandles and removed suspended Euribor/Libor indexes
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YC1YBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YC1YBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="DayCounter">'General Settings'!$D$19</definedName>
     <definedName name="DepoInclusionCriteria">Selected!$B$5</definedName>
     <definedName name="Discounting">'General Settings'!$L$15</definedName>
-    <definedName name="Discounting2">'General Settings'!$L$16</definedName>
+    <definedName name="Discounting2">'General Settings'!#REF!</definedName>
     <definedName name="DiscountingCurve" localSheetId="5">'1Y_SwapsFromBasis'!$L$2</definedName>
     <definedName name="FamilyName">'General Settings'!$L$11</definedName>
     <definedName name="FileOverwrite">'General Settings'!$L$6</definedName>
@@ -768,9 +768,6 @@
     <t>Fwd start</t>
   </si>
   <si>
-    <t>Discounting2</t>
-  </si>
-  <si>
     <t>Discounting</t>
   </si>
   <si>
@@ -793,6 +790,9 @@
   </si>
   <si>
     <t>EUR_YCRH_SwapsFromBasis</t>
+  </si>
+  <si>
+    <t>EUR1Y</t>
   </si>
 </sst>
 </file>
@@ -1867,21 +1867,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1899,6 +1884,21 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2214,42 +2214,44 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="2.7109375" style="194" customWidth="1"/>
-    <col min="3" max="3" width="18" style="194" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="194" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="2.7109375" style="194" customWidth="1"/>
-    <col min="7" max="7" width="4" style="194" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.28515625" style="194" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="2.7109375" style="194" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="194" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53.7109375" style="194" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.7109375" style="194" customWidth="1"/>
-    <col min="14" max="16384" width="8" style="194"/>
+    <col min="1" max="2" width="2.7109375" style="189" customWidth="1"/>
+    <col min="3" max="3" width="18" style="189" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="189" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="2.7109375" style="189" customWidth="1"/>
+    <col min="7" max="7" width="4" style="189" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.28515625" style="189" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="2.7109375" style="189" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="189" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53.7109375" style="189" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" style="189" customWidth="1"/>
+    <col min="14" max="16384" width="8" style="189"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="194" t="str">
+      <c r="B1" s="189" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Feb  7 2014 15:33:58</v>
+        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Mar  3 2014 10:58:57</v>
       </c>
     </row>
     <row r="2" spans="2:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="203"/>
-      <c r="D2" s="203"/>
-      <c r="E2" s="204"/>
-      <c r="J2" s="202" t="s">
+      <c r="C2" s="198"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="199"/>
+      <c r="J2" s="197" t="s">
         <v>170</v>
       </c>
-      <c r="K2" s="203"/>
-      <c r="L2" s="203"/>
-      <c r="M2" s="205"/>
+      <c r="K2" s="198"/>
+      <c r="L2" s="198"/>
+      <c r="M2" s="200"/>
     </row>
     <row r="3" spans="2:13" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="61"/>
@@ -2270,10 +2272,10 @@
         <v>112</v>
       </c>
       <c r="E4" s="57"/>
-      <c r="G4" s="196" t="s">
+      <c r="G4" s="191" t="s">
         <v>114</v>
       </c>
-      <c r="H4" s="197"/>
+      <c r="H4" s="192"/>
       <c r="J4" s="123"/>
       <c r="K4" s="122" t="s">
         <v>169</v>
@@ -2292,10 +2294,10 @@
         <v>12</v>
       </c>
       <c r="E5" s="57"/>
-      <c r="G5" s="198" t="s">
+      <c r="G5" s="193" t="s">
         <v>112</v>
       </c>
-      <c r="H5" s="199" t="s">
+      <c r="H5" s="194" t="s">
         <v>111</v>
       </c>
       <c r="J5" s="123"/>
@@ -2304,7 +2306,7 @@
       </c>
       <c r="L5" s="124" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\Users\erik\Documents\repos\quantlib\QuantLibXL\Data2\XML\</v>
+        <v>C:\Projects\quantlib\QuantLibXL\Data2\XML\</v>
       </c>
       <c r="M5" s="121"/>
     </row>
@@ -2318,10 +2320,10 @@
         <v>1Y</v>
       </c>
       <c r="E6" s="57"/>
-      <c r="G6" s="198" t="s">
+      <c r="G6" s="193" t="s">
         <v>109</v>
       </c>
-      <c r="H6" s="199"/>
+      <c r="H6" s="194"/>
       <c r="J6" s="123"/>
       <c r="K6" s="122" t="s">
         <v>167</v>
@@ -2341,10 +2343,10 @@
         <v>12E</v>
       </c>
       <c r="E7" s="57"/>
-      <c r="G7" s="198" t="s">
+      <c r="G7" s="193" t="s">
         <v>107</v>
       </c>
-      <c r="H7" s="199"/>
+      <c r="H7" s="194"/>
       <c r="J7" s="120"/>
       <c r="K7" s="119"/>
       <c r="L7" s="119"/>
@@ -2360,16 +2362,16 @@
         <v>AB</v>
       </c>
       <c r="E8" s="57"/>
-      <c r="G8" s="200" t="s">
+      <c r="G8" s="195" t="s">
         <v>105</v>
       </c>
-      <c r="H8" s="201" t="s">
+      <c r="H8" s="196" t="s">
         <v>104</v>
       </c>
-      <c r="J8" s="195"/>
-      <c r="K8" s="195"/>
-      <c r="L8" s="195"/>
-      <c r="M8" s="195"/>
+      <c r="J8" s="190"/>
+      <c r="K8" s="190"/>
+      <c r="L8" s="190"/>
+      <c r="M8" s="190"/>
     </row>
     <row r="9" spans="2:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="61"/>
@@ -2381,12 +2383,12 @@
         <v>EUR_YC1YRH</v>
       </c>
       <c r="E9" s="57"/>
-      <c r="J9" s="202" t="s">
+      <c r="J9" s="197" t="s">
         <v>166</v>
       </c>
-      <c r="K9" s="203"/>
-      <c r="L9" s="203"/>
-      <c r="M9" s="205"/>
+      <c r="K9" s="198"/>
+      <c r="L9" s="198"/>
+      <c r="M9" s="200"/>
     </row>
     <row r="10" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="61"/>
@@ -2408,7 +2410,7 @@
         <v>101</v>
       </c>
       <c r="D11" s="80">
-        <v>41684.573217592595</v>
+        <v>41702.442187499997</v>
       </c>
       <c r="E11" s="57"/>
       <c r="J11" s="115"/>
@@ -2445,10 +2447,10 @@
       <c r="E13" s="57"/>
       <c r="J13" s="115"/>
       <c r="K13" s="114" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L13" s="116" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M13" s="112"/>
     </row>
@@ -2459,15 +2461,15 @@
       </c>
       <c r="D14" s="77" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(#REF!),NA(),#REF!),IF(ISERROR(#REF!),NA(),#REF!),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_EURYC1Y#0002</v>
+        <v>_EURYC1Y#0001</v>
       </c>
       <c r="E14" s="57"/>
       <c r="J14" s="115"/>
       <c r="K14" s="114" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L14" s="116" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M14" s="112"/>
     </row>
@@ -2483,15 +2485,15 @@
       <c r="E15" s="57"/>
       <c r="J15" s="115"/>
       <c r="K15" s="114" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L15" s="113" t="str">
-        <f>PROPER(Currency)&amp;"YC"</f>
-        <v>EurYC</v>
+        <f>PROPER(Currency)&amp;"ON"</f>
+        <v>EurON</v>
       </c>
       <c r="M15" s="112"/>
     </row>
-    <row r="16" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="61"/>
       <c r="C16" s="75" t="s">
         <v>98</v>
@@ -2501,17 +2503,12 @@
         <v>_EURYC1Y</v>
       </c>
       <c r="E16" s="57"/>
-      <c r="J16" s="115"/>
-      <c r="K16" s="114" t="s">
-        <v>183</v>
-      </c>
-      <c r="L16" s="113" t="str">
-        <f>PROPER(Currency)&amp;"YCSTD"</f>
-        <v>EurYCSTD</v>
-      </c>
-      <c r="M16" s="112"/>
-    </row>
-    <row r="17" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="111"/>
+      <c r="K16" s="110"/>
+      <c r="L16" s="110"/>
+      <c r="M16" s="109"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="61"/>
       <c r="C17" s="70" t="s">
         <v>97</v>
@@ -2520,12 +2517,8 @@
         <v>2</v>
       </c>
       <c r="E17" s="57"/>
-      <c r="J17" s="111"/>
-      <c r="K17" s="110"/>
-      <c r="L17" s="110"/>
-      <c r="M17" s="109"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="61"/>
       <c r="C18" s="70" t="s">
         <v>96</v>
@@ -2535,7 +2528,7 @@
       </c>
       <c r="E18" s="57"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="61"/>
       <c r="C19" s="70" t="s">
         <v>94</v>
@@ -2543,7 +2536,7 @@
       <c r="D19" s="72"/>
       <c r="E19" s="57"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="61"/>
       <c r="C20" s="70" t="s">
         <v>93</v>
@@ -2554,7 +2547,7 @@
       </c>
       <c r="E20" s="57"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="61"/>
       <c r="C21" s="70" t="s">
         <v>92</v>
@@ -2564,7 +2557,7 @@
       </c>
       <c r="E21" s="57"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="61"/>
       <c r="C22" s="68" t="s">
         <v>90</v>
@@ -2574,17 +2567,17 @@
       </c>
       <c r="E22" s="57"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="61"/>
       <c r="C23" s="66"/>
       <c r="D23" s="66"/>
       <c r="E23" s="57"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="61"/>
       <c r="C24" s="65">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="D24" s="64">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
@@ -2592,19 +2585,19 @@
       </c>
       <c r="E24" s="57"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="61"/>
       <c r="C25" s="63">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>63604</v>
+        <v>63619</v>
       </c>
       <c r="D25" s="62">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.18144476455568445</v>
+        <v>0.20316032572374745</v>
       </c>
       <c r="E25" s="57"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="61"/>
       <c r="C26" s="60" t="s">
         <v>80</v>
@@ -2615,10 +2608,15 @@
       </c>
       <c r="E26" s="57"/>
     </row>
-    <row r="27" spans="2:13" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="56"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
+      <c r="C27" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="55" t="b">
+        <f>_xll.qlRelinkableHandleLinkTo(C27,YieldCurve)</f>
+        <v>1</v>
+      </c>
       <c r="E27" s="54"/>
     </row>
   </sheetData>
@@ -2688,11 +2686,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B1" s="189" t="s">
+      <c r="B1" s="201" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="190"/>
-      <c r="D1" s="191"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="203"/>
       <c r="E1" s="31" t="s">
         <v>78</v>
       </c>
@@ -2822,11 +2820,11 @@
       </c>
       <c r="K4" s="11">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L4" s="10">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41689</v>
+        <v>41705</v>
       </c>
       <c r="M4" s="1">
         <v>30</v>
@@ -2861,11 +2859,11 @@
       </c>
       <c r="K5" s="11">
         <f>_xll.qlRateHelperEarliestDate($E5,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L5" s="10">
         <f>_xll.qlRateHelperLatestDate($E5,Trigger)</f>
-        <v>41695</v>
+        <v>41711</v>
       </c>
       <c r="M5" s="1">
         <v>40</v>
@@ -2900,11 +2898,11 @@
       </c>
       <c r="K6" s="11">
         <f>_xll.qlRateHelperEarliestDate($E6,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L6" s="10">
         <f>_xll.qlRateHelperLatestDate($E6,Trigger)</f>
-        <v>41702</v>
+        <v>41718</v>
       </c>
       <c r="M6" s="1">
         <v>50</v>
@@ -2939,11 +2937,11 @@
       </c>
       <c r="K7" s="11">
         <f>_xll.qlRateHelperEarliestDate($E7,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L7" s="10">
         <f>_xll.qlRateHelperLatestDate($E7,Trigger)</f>
-        <v>41709</v>
+        <v>41725</v>
       </c>
       <c r="M7" s="1">
         <v>60</v>
@@ -2978,11 +2976,11 @@
       </c>
       <c r="K8" s="11">
         <f>_xll.qlRateHelperEarliestDate($E8,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L8" s="10">
         <f>_xll.qlRateHelperLatestDate($E8,Trigger)</f>
-        <v>41716</v>
+        <v>41736</v>
       </c>
       <c r="M8" s="1">
         <v>70</v>
@@ -3017,11 +3015,11 @@
       </c>
       <c r="K9" s="11">
         <f>_xll.qlRateHelperEarliestDate($E9,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L9" s="10">
         <f>_xll.qlRateHelperLatestDate($E9,Trigger)</f>
-        <v>41751</v>
+        <v>41765</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
@@ -3050,11 +3048,11 @@
       </c>
       <c r="K10" s="11">
         <f>_xll.qlRateHelperEarliestDate($E10,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L10" s="10">
         <f>_xll.qlRateHelperLatestDate($E10,Trigger)</f>
-        <v>41778</v>
+        <v>41796</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
@@ -3083,11 +3081,11 @@
       </c>
       <c r="K11" s="11">
         <f>_xll.qlRateHelperEarliestDate($E11,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L11" s="10">
         <f>_xll.qlRateHelperLatestDate($E11,Trigger)</f>
-        <v>41808</v>
+        <v>41827</v>
       </c>
       <c r="M11" s="1">
         <v>7</v>
@@ -3119,11 +3117,11 @@
       </c>
       <c r="K12" s="11">
         <f>_xll.qlRateHelperEarliestDate($E12,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L12" s="10">
         <f>_xll.qlRateHelperLatestDate($E12,Trigger)</f>
-        <v>41838</v>
+        <v>41857</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
@@ -3152,11 +3150,11 @@
       </c>
       <c r="K13" s="11">
         <f>_xll.qlRateHelperEarliestDate($E13,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L13" s="10">
         <f>_xll.qlRateHelperLatestDate($E13,Trigger)</f>
-        <v>41869</v>
+        <v>41890</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
@@ -3185,11 +3183,11 @@
       </c>
       <c r="K14" s="11">
         <f>_xll.qlRateHelperEarliestDate($E14,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L14" s="10">
         <f>_xll.qlRateHelperLatestDate($E14,Trigger)</f>
-        <v>41900</v>
+        <v>41918</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
@@ -3218,11 +3216,11 @@
       </c>
       <c r="K15" s="11">
         <f>_xll.qlRateHelperEarliestDate($E15,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L15" s="10">
         <f>_xll.qlRateHelperLatestDate($E15,Trigger)</f>
-        <v>41932</v>
+        <v>41949</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
@@ -3251,11 +3249,11 @@
       </c>
       <c r="K16" s="11">
         <f>_xll.qlRateHelperEarliestDate($E16,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L16" s="10">
         <f>_xll.qlRateHelperLatestDate($E16,Trigger)</f>
-        <v>41961</v>
+        <v>41981</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
@@ -3284,11 +3282,11 @@
       </c>
       <c r="K17" s="11">
         <f>_xll.qlRateHelperEarliestDate($E17,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L17" s="10">
         <f>_xll.qlRateHelperLatestDate($E17,Trigger)</f>
-        <v>41991</v>
+        <v>42010</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
@@ -3317,11 +3315,11 @@
       </c>
       <c r="K18" s="11">
         <f>_xll.qlRateHelperEarliestDate($E18,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L18" s="10">
         <f>_xll.qlRateHelperLatestDate($E18,Trigger)</f>
-        <v>42023</v>
+        <v>42041</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
@@ -3350,11 +3348,11 @@
       </c>
       <c r="K19" s="4">
         <f>_xll.qlRateHelperEarliestDate($E19,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L19" s="3">
         <f>_xll.qlRateHelperLatestDate($E19,Trigger)</f>
-        <v>42053</v>
+        <v>42069</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
@@ -3388,11 +3386,11 @@
       </c>
       <c r="K20" s="19">
         <f>_xll.qlRateHelperEarliestDate($E20,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L20" s="18">
         <f>_xll.qlRateHelperLatestDate($E20,Trigger)</f>
-        <v>42053</v>
+        <v>42069</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
@@ -3426,11 +3424,11 @@
       </c>
       <c r="K21" s="4">
         <f>_xll.qlRateHelperEarliestDate($E21,Trigger)</f>
-        <v>41689</v>
+        <v>41705</v>
       </c>
       <c r="L21" s="3">
         <f>_xll.qlRateHelperLatestDate($E21,Trigger)</f>
-        <v>42054</v>
+        <v>42072</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
@@ -3464,11 +3462,11 @@
       </c>
       <c r="K22" s="11">
         <f>_xll.qlRateHelperEarliestDate($E22,Trigger)</f>
-        <v>41716</v>
+        <v>41736</v>
       </c>
       <c r="L22" s="10">
         <f>_xll.qlRateHelperLatestDate($E22,Trigger)</f>
-        <v>42081</v>
+        <v>42101</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
@@ -3502,11 +3500,11 @@
       </c>
       <c r="K23" s="11">
         <f>_xll.qlRateHelperEarliestDate($E23,Trigger)</f>
-        <v>41751</v>
+        <v>41765</v>
       </c>
       <c r="L23" s="10">
         <f>_xll.qlRateHelperLatestDate($E23,Trigger)</f>
-        <v>42116</v>
+        <v>42130</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
@@ -3540,11 +3538,11 @@
       </c>
       <c r="K24" s="11">
         <f>_xll.qlRateHelperEarliestDate($E24,Trigger)</f>
-        <v>41778</v>
+        <v>41796</v>
       </c>
       <c r="L24" s="10">
         <f>_xll.qlRateHelperLatestDate($E24,Trigger)</f>
-        <v>42143</v>
+        <v>42163</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
@@ -3578,11 +3576,11 @@
       </c>
       <c r="K25" s="11">
         <f>_xll.qlRateHelperEarliestDate($E25,Trigger)</f>
-        <v>41808</v>
+        <v>41827</v>
       </c>
       <c r="L25" s="10">
         <f>_xll.qlRateHelperLatestDate($E25,Trigger)</f>
-        <v>42173</v>
+        <v>42192</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
@@ -3616,11 +3614,11 @@
       </c>
       <c r="K26" s="11">
         <f>_xll.qlRateHelperEarliestDate($E26,Trigger)</f>
-        <v>41838</v>
+        <v>41857</v>
       </c>
       <c r="L26" s="10">
         <f>_xll.qlRateHelperLatestDate($E26,Trigger)</f>
-        <v>42205</v>
+        <v>42222</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
@@ -3654,11 +3652,11 @@
       </c>
       <c r="K27" s="11">
         <f>_xll.qlRateHelperEarliestDate($E27,Trigger)</f>
-        <v>41869</v>
+        <v>41890</v>
       </c>
       <c r="L27" s="10">
         <f>_xll.qlRateHelperLatestDate($E27,Trigger)</f>
-        <v>42234</v>
+        <v>42255</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
@@ -3692,11 +3690,11 @@
       </c>
       <c r="K28" s="11">
         <f>_xll.qlRateHelperEarliestDate($E28,Trigger)</f>
-        <v>41900</v>
+        <v>41918</v>
       </c>
       <c r="L28" s="10">
         <f>_xll.qlRateHelperLatestDate($E28,Trigger)</f>
-        <v>42265</v>
+        <v>42283</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
@@ -3730,11 +3728,11 @@
       </c>
       <c r="K29" s="11">
         <f>_xll.qlRateHelperEarliestDate($E29,Trigger)</f>
-        <v>41932</v>
+        <v>41949</v>
       </c>
       <c r="L29" s="10">
         <f>_xll.qlRateHelperLatestDate($E29,Trigger)</f>
-        <v>42297</v>
+        <v>42314</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
@@ -3768,11 +3766,11 @@
       </c>
       <c r="K30" s="11">
         <f>_xll.qlRateHelperEarliestDate($E30,Trigger)</f>
-        <v>41961</v>
+        <v>41981</v>
       </c>
       <c r="L30" s="10">
         <f>_xll.qlRateHelperLatestDate($E30,Trigger)</f>
-        <v>42326</v>
+        <v>42346</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
@@ -3806,11 +3804,11 @@
       </c>
       <c r="K31" s="11">
         <f>_xll.qlRateHelperEarliestDate($E31,Trigger)</f>
-        <v>41991</v>
+        <v>42010</v>
       </c>
       <c r="L31" s="10">
         <f>_xll.qlRateHelperLatestDate($E31,Trigger)</f>
-        <v>42356</v>
+        <v>42375</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
@@ -3844,11 +3842,11 @@
       </c>
       <c r="K32" s="11">
         <f>_xll.qlRateHelperEarliestDate($E32,Trigger)</f>
-        <v>42023</v>
+        <v>42041</v>
       </c>
       <c r="L32" s="10">
         <f>_xll.qlRateHelperLatestDate($E32,Trigger)</f>
-        <v>42388</v>
+        <v>42408</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -3868,7 +3866,7 @@
       </c>
       <c r="F33" s="13">
         <f>_xll.qlRateHelperQuoteValue($E33,Trigger)</f>
-        <v>6.7400000000000003E-3</v>
+        <v>6.3899999999999998E-3</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="12" t="b">
@@ -3882,11 +3880,11 @@
       </c>
       <c r="K33" s="11">
         <f>_xll.qlRateHelperEarliestDate($E33,Trigger)</f>
-        <v>42053</v>
+        <v>42069</v>
       </c>
       <c r="L33" s="10">
         <f>_xll.qlRateHelperLatestDate($E33,Trigger)</f>
-        <v>42418</v>
+        <v>42436</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -3920,11 +3918,11 @@
       </c>
       <c r="K34" s="11">
         <f>_xll.qlRateHelperEarliestDate($E34,Trigger)</f>
-        <v>42081</v>
+        <v>42101</v>
       </c>
       <c r="L34" s="10">
         <f>_xll.qlRateHelperLatestDate($E34,Trigger)</f>
-        <v>42447</v>
+        <v>42467</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -3958,11 +3956,11 @@
       </c>
       <c r="K35" s="11">
         <f>_xll.qlRateHelperEarliestDate($E35,Trigger)</f>
-        <v>42114</v>
+        <v>42130</v>
       </c>
       <c r="L35" s="10">
         <f>_xll.qlRateHelperLatestDate($E35,Trigger)</f>
-        <v>42480</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -3996,11 +3994,11 @@
       </c>
       <c r="K36" s="11">
         <f>_xll.qlRateHelperEarliestDate($E36,Trigger)</f>
-        <v>42142</v>
+        <v>42163</v>
       </c>
       <c r="L36" s="10">
         <f>_xll.qlRateHelperLatestDate($E36,Trigger)</f>
-        <v>42508</v>
+        <v>42529</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -4034,11 +4032,11 @@
       </c>
       <c r="K37" s="11">
         <f>_xll.qlRateHelperEarliestDate($E37,Trigger)</f>
-        <v>42173</v>
+        <v>42191</v>
       </c>
       <c r="L37" s="10">
         <f>_xll.qlRateHelperLatestDate($E37,Trigger)</f>
-        <v>42541</v>
+        <v>42557</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -4072,11 +4070,11 @@
       </c>
       <c r="K38" s="11">
         <f>_xll.qlRateHelperEarliestDate($E38,Trigger)</f>
-        <v>42205</v>
+        <v>42222</v>
       </c>
       <c r="L38" s="10">
         <f>_xll.qlRateHelperLatestDate($E38,Trigger)</f>
-        <v>42571</v>
+        <v>42590</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -4110,11 +4108,11 @@
       </c>
       <c r="K39" s="4">
         <f>_xll.qlRateHelperEarliestDate($E39,Trigger)</f>
-        <v>42234</v>
+        <v>42254</v>
       </c>
       <c r="L39" s="3">
         <f>_xll.qlRateHelperLatestDate($E39,Trigger)</f>
-        <v>42600</v>
+        <v>42620</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="11.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4128,11 +4126,11 @@
       </c>
       <c r="D40" s="14" t="str">
         <f t="array" ref="D40:D81">_xll.qlIMMNextCodes(_xll.qlSettingsEvaluationDate(Trigger)-1,$A40:$A81)</f>
-        <v>G4</v>
+        <v>H4</v>
       </c>
       <c r="E40" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YG4</v>
+        <v>EUR_YC1YRH_FUT1YH4</v>
       </c>
       <c r="F40" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
@@ -4170,11 +4168,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D41" s="14" t="str">
-        <v>H4</v>
+        <v>J4</v>
       </c>
       <c r="E41" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YH4</v>
+        <v>EUR_YC1YRH_FUT1YJ4</v>
       </c>
       <c r="F41" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
@@ -4212,11 +4210,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D42" s="14" t="str">
-        <v>J4</v>
+        <v>K4</v>
       </c>
       <c r="E42" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YJ4</v>
+        <v>EUR_YC1YRH_FUT1YK4</v>
       </c>
       <c r="F42" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
@@ -4254,11 +4252,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D43" s="14" t="str">
-        <v>K4</v>
+        <v>M4</v>
       </c>
       <c r="E43" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YK4</v>
+        <v>EUR_YC1YRH_FUT1YM4</v>
       </c>
       <c r="F43" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
@@ -4296,11 +4294,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D44" s="14" t="str">
-        <v>M4</v>
+        <v>N4</v>
       </c>
       <c r="E44" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YM4</v>
+        <v>EUR_YC1YRH_FUT1YN4</v>
       </c>
       <c r="F44" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
@@ -4338,11 +4336,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D45" s="14" t="str">
-        <v>N4</v>
+        <v>Q4</v>
       </c>
       <c r="E45" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YN4</v>
+        <v>EUR_YC1YRH_FUT1YQ4</v>
       </c>
       <c r="F45" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
@@ -4380,11 +4378,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D46" s="14" t="str">
-        <v>Q4</v>
+        <v>U4</v>
       </c>
       <c r="E46" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YQ4</v>
+        <v>EUR_YC1YRH_FUT1YU4</v>
       </c>
       <c r="F46" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
@@ -4422,11 +4420,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D47" s="14" t="str">
-        <v>U4</v>
+        <v>V4</v>
       </c>
       <c r="E47" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YU4</v>
+        <v>EUR_YC1YRH_FUT1YV4</v>
       </c>
       <c r="F47" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
@@ -4464,11 +4462,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D48" s="14" t="str">
-        <v>V4</v>
+        <v>X4</v>
       </c>
       <c r="E48" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YV4</v>
+        <v>EUR_YC1YRH_FUT1YX4</v>
       </c>
       <c r="F48" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E48,Trigger)</f>
@@ -4506,11 +4504,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D49" s="14" t="str">
-        <v>X4</v>
+        <v>Z4</v>
       </c>
       <c r="E49" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YX4</v>
+        <v>EUR_YC1YRH_FUT1YZ4</v>
       </c>
       <c r="F49" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E49,Trigger)</f>
@@ -4548,11 +4546,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D50" s="14" t="str">
-        <v>Z4</v>
+        <v>F5</v>
       </c>
       <c r="E50" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YZ4</v>
+        <v>EUR_YC1YRH_FUT1YF5</v>
       </c>
       <c r="F50" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E50,Trigger)</f>
@@ -4590,11 +4588,11 @@
         <v>FUT1Y</v>
       </c>
       <c r="D51" s="14" t="str">
-        <v>F5</v>
+        <v>G5</v>
       </c>
       <c r="E51" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>EUR_YC1YRH_FUT1YF5</v>
+        <v>EUR_YC1YRH_FUT1YG5</v>
       </c>
       <c r="F51" s="28" t="e">
         <f>_xll.qlRateHelperQuoteValue($E51,Trigger)</f>
@@ -8289,7 +8287,7 @@
       </c>
       <c r="F137" s="13">
         <f>_xll.qlRateHelperQuoteValue($E137,Trigger)</f>
-        <v>5.7800000000000004E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="G137" s="13">
         <f>_xll.qlSwapRateHelperSpread($E137,Trigger)</f>
@@ -8306,11 +8304,11 @@
       </c>
       <c r="K137" s="11">
         <f>_xll.qlRateHelperEarliestDate($E137,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L137" s="10">
         <f>_xll.qlRateHelperLatestDate($E137,Trigger)</f>
-        <v>42053</v>
+        <v>42069</v>
       </c>
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.2">
@@ -8331,7 +8329,7 @@
       </c>
       <c r="F138" s="13">
         <f>_xll.qlRateHelperQuoteValue($E138,Trigger)</f>
-        <v>5.5640000000000004E-3</v>
+        <v>5.3790000000000001E-3</v>
       </c>
       <c r="G138" s="13">
         <f>_xll.qlSwapRateHelperSpread($E138,Trigger)</f>
@@ -8348,11 +8346,11 @@
       </c>
       <c r="K138" s="11">
         <f>_xll.qlRateHelperEarliestDate($E138,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L138" s="10">
         <f>_xll.qlRateHelperLatestDate($E138,Trigger)</f>
-        <v>42142</v>
+        <v>42163</v>
       </c>
     </row>
     <row r="139" spans="2:14" x14ac:dyDescent="0.2">
@@ -8373,7 +8371,7 @@
       </c>
       <c r="F139" s="13">
         <f>_xll.qlRateHelperQuoteValue($E139,Trigger)</f>
-        <v>5.8820000000000001E-3</v>
+        <v>5.7210000000000004E-3</v>
       </c>
       <c r="G139" s="13">
         <f>_xll.qlSwapRateHelperSpread($E139,Trigger)</f>
@@ -8390,11 +8388,11 @@
       </c>
       <c r="K139" s="11">
         <f>_xll.qlRateHelperEarliestDate($E139,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L139" s="10">
         <f>_xll.qlRateHelperLatestDate($E139,Trigger)</f>
-        <v>42234</v>
+        <v>42254</v>
       </c>
     </row>
     <row r="140" spans="2:14" x14ac:dyDescent="0.2">
@@ -8415,7 +8413,7 @@
       </c>
       <c r="F140" s="13">
         <f>_xll.qlRateHelperQuoteValue($E140,Trigger)</f>
-        <v>5.8760000000000001E-3</v>
+        <v>5.6559999999999996E-3</v>
       </c>
       <c r="G140" s="13">
         <f>_xll.qlSwapRateHelperSpread($E140,Trigger)</f>
@@ -8432,11 +8430,11 @@
       </c>
       <c r="K140" s="11">
         <f>_xll.qlRateHelperEarliestDate($E140,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L140" s="10">
         <f>_xll.qlRateHelperLatestDate($E140,Trigger)</f>
-        <v>42326</v>
+        <v>42345</v>
       </c>
     </row>
     <row r="141" spans="2:14" x14ac:dyDescent="0.2">
@@ -8457,7 +8455,7 @@
       </c>
       <c r="F141" s="13">
         <f>_xll.qlRateHelperQuoteValue($E141,Trigger)</f>
-        <v>6.3E-3</v>
+        <v>6.0499999999999998E-3</v>
       </c>
       <c r="G141" s="13">
         <f>_xll.qlSwapRateHelperSpread($E141,Trigger)</f>
@@ -8474,11 +8472,11 @@
       </c>
       <c r="K141" s="11">
         <f>_xll.qlRateHelperEarliestDate($E141,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L141" s="10">
         <f>_xll.qlRateHelperLatestDate($E141,Trigger)</f>
-        <v>42418</v>
+        <v>42436</v>
       </c>
     </row>
     <row r="142" spans="2:14" x14ac:dyDescent="0.2">
@@ -8499,7 +8497,7 @@
       </c>
       <c r="F142" s="13">
         <f>_xll.qlRateHelperQuoteValue($E142,Trigger)</f>
-        <v>7.9900000000000006E-3</v>
+        <v>7.4800000000000005E-3</v>
       </c>
       <c r="G142" s="13">
         <f>_xll.qlSwapRateHelperSpread($E142,Trigger)</f>
@@ -8516,11 +8514,11 @@
       </c>
       <c r="K142" s="11">
         <f>_xll.qlRateHelperEarliestDate($E142,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L142" s="10">
         <f>_xll.qlRateHelperLatestDate($E142,Trigger)</f>
-        <v>42786</v>
+        <v>42800</v>
       </c>
     </row>
     <row r="143" spans="2:14" x14ac:dyDescent="0.2">
@@ -8541,7 +8539,7 @@
       </c>
       <c r="F143" s="13">
         <f>_xll.qlRateHelperQuoteValue($E143,Trigger)</f>
-        <v>1.027E-2</v>
+        <v>9.4500000000000001E-3</v>
       </c>
       <c r="G143" s="13">
         <f>_xll.qlSwapRateHelperSpread($E143,Trigger)</f>
@@ -8558,11 +8556,11 @@
       </c>
       <c r="K143" s="11">
         <f>_xll.qlRateHelperEarliestDate($E143,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L143" s="10">
         <f>_xll.qlRateHelperLatestDate($E143,Trigger)</f>
-        <v>43150</v>
+        <v>43165</v>
       </c>
     </row>
     <row r="144" spans="2:14" x14ac:dyDescent="0.2">
@@ -8583,7 +8581,7 @@
       </c>
       <c r="F144" s="13">
         <f>_xll.qlRateHelperQuoteValue($E144,Trigger)</f>
-        <v>1.2610000000000001E-2</v>
+        <v>1.149E-2</v>
       </c>
       <c r="G144" s="13">
         <f>_xll.qlSwapRateHelperSpread($E144,Trigger)</f>
@@ -8600,11 +8598,11 @@
       </c>
       <c r="K144" s="11">
         <f>_xll.qlRateHelperEarliestDate($E144,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L144" s="10">
         <f>_xll.qlRateHelperLatestDate($E144,Trigger)</f>
-        <v>43514</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.2">
@@ -8625,7 +8623,7 @@
       </c>
       <c r="F145" s="13">
         <f>_xll.qlRateHelperQuoteValue($E145,Trigger)</f>
-        <v>1.4789999999999999E-2</v>
+        <v>1.345E-2</v>
       </c>
       <c r="G145" s="13">
         <f>_xll.qlSwapRateHelperSpread($E145,Trigger)</f>
@@ -8642,11 +8640,11 @@
       </c>
       <c r="K145" s="11">
         <f>_xll.qlRateHelperEarliestDate($E145,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L145" s="10">
         <f>_xll.qlRateHelperLatestDate($E145,Trigger)</f>
-        <v>43879</v>
+        <v>43896</v>
       </c>
     </row>
     <row r="146" spans="2:12" x14ac:dyDescent="0.2">
@@ -8667,7 +8665,7 @@
       </c>
       <c r="F146" s="13">
         <f>_xll.qlRateHelperQuoteValue($E146,Trigger)</f>
-        <v>1.677E-2</v>
+        <v>1.5269999999999999E-2</v>
       </c>
       <c r="G146" s="13">
         <f>_xll.qlSwapRateHelperSpread($E146,Trigger)</f>
@@ -8684,11 +8682,11 @@
       </c>
       <c r="K146" s="11">
         <f>_xll.qlRateHelperEarliestDate($E146,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L146" s="10">
         <f>_xll.qlRateHelperLatestDate($E146,Trigger)</f>
-        <v>44245</v>
+        <v>44263</v>
       </c>
     </row>
     <row r="147" spans="2:12" x14ac:dyDescent="0.2">
@@ -8709,7 +8707,7 @@
       </c>
       <c r="F147" s="13">
         <f>_xll.qlRateHelperQuoteValue($E147,Trigger)</f>
-        <v>1.8540000000000001E-2</v>
+        <v>1.6910000000000001E-2</v>
       </c>
       <c r="G147" s="13">
         <f>_xll.qlSwapRateHelperSpread($E147,Trigger)</f>
@@ -8726,11 +8724,11 @@
       </c>
       <c r="K147" s="11">
         <f>_xll.qlRateHelperEarliestDate($E147,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L147" s="10">
         <f>_xll.qlRateHelperLatestDate($E147,Trigger)</f>
-        <v>44610</v>
+        <v>44627</v>
       </c>
     </row>
     <row r="148" spans="2:12" x14ac:dyDescent="0.2">
@@ -8751,7 +8749,7 @@
       </c>
       <c r="F148" s="13">
         <f>_xll.qlRateHelperQuoteValue($E148,Trigger)</f>
-        <v>2.0110000000000003E-2</v>
+        <v>1.8380000000000001E-2</v>
       </c>
       <c r="G148" s="13">
         <f>_xll.qlSwapRateHelperSpread($E148,Trigger)</f>
@@ -8768,11 +8766,11 @@
       </c>
       <c r="K148" s="11">
         <f>_xll.qlRateHelperEarliestDate($E148,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L148" s="10">
         <f>_xll.qlRateHelperLatestDate($E148,Trigger)</f>
-        <v>44977</v>
+        <v>44991</v>
       </c>
     </row>
     <row r="149" spans="2:12" x14ac:dyDescent="0.2">
@@ -8793,7 +8791,7 @@
       </c>
       <c r="F149" s="13">
         <f>_xll.qlRateHelperQuoteValue($E149,Trigger)</f>
-        <v>2.147E-2</v>
+        <v>1.9700000000000002E-2</v>
       </c>
       <c r="G149" s="13">
         <f>_xll.qlSwapRateHelperSpread($E149,Trigger)</f>
@@ -8810,11 +8808,11 @@
       </c>
       <c r="K149" s="11">
         <f>_xll.qlRateHelperEarliestDate($E149,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L149" s="10">
         <f>_xll.qlRateHelperLatestDate($E149,Trigger)</f>
-        <v>45341</v>
+        <v>45357</v>
       </c>
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.2">
@@ -8835,7 +8833,7 @@
       </c>
       <c r="F150" s="13">
         <f>_xll.qlRateHelperQuoteValue($E150,Trigger)</f>
-        <v>2.2639999999999997E-2</v>
+        <v>2.0840000000000001E-2</v>
       </c>
       <c r="G150" s="13">
         <f>_xll.qlSwapRateHelperSpread($E150,Trigger)</f>
@@ -8852,11 +8850,11 @@
       </c>
       <c r="K150" s="11">
         <f>_xll.qlRateHelperEarliestDate($E150,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L150" s="10">
         <f>_xll.qlRateHelperLatestDate($E150,Trigger)</f>
-        <v>45706</v>
+        <v>45722</v>
       </c>
     </row>
     <row r="151" spans="2:12" x14ac:dyDescent="0.2">
@@ -8877,7 +8875,7 @@
       </c>
       <c r="F151" s="13">
         <f>_xll.qlRateHelperQuoteValue($E151,Trigger)</f>
-        <v>2.3640000000000001E-2</v>
+        <v>2.1789999999999997E-2</v>
       </c>
       <c r="G151" s="13">
         <f>_xll.qlSwapRateHelperSpread($E151,Trigger)</f>
@@ -8894,11 +8892,11 @@
       </c>
       <c r="K151" s="11">
         <f>_xll.qlRateHelperEarliestDate($E151,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L151" s="10">
         <f>_xll.qlRateHelperLatestDate($E151,Trigger)</f>
-        <v>46071</v>
+        <v>46087</v>
       </c>
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.2">
@@ -8919,7 +8917,7 @@
       </c>
       <c r="F152" s="13">
         <f>_xll.qlRateHelperQuoteValue($E152,Trigger)</f>
-        <v>2.4482E-2</v>
+        <v>2.2615E-2</v>
       </c>
       <c r="G152" s="13">
         <f>_xll.qlSwapRateHelperSpread($E152,Trigger)</f>
@@ -8936,11 +8934,11 @@
       </c>
       <c r="K152" s="11">
         <f>_xll.qlRateHelperEarliestDate($E152,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L152" s="10">
         <f>_xll.qlRateHelperLatestDate($E152,Trigger)</f>
-        <v>46436</v>
+        <v>46454</v>
       </c>
     </row>
     <row r="153" spans="2:12" x14ac:dyDescent="0.2">
@@ -8961,7 +8959,7 @@
       </c>
       <c r="F153" s="13">
         <f>_xll.qlRateHelperQuoteValue($E153,Trigger)</f>
-        <v>2.5179E-2</v>
+        <v>2.3309999999999997E-2</v>
       </c>
       <c r="G153" s="13">
         <f>_xll.qlSwapRateHelperSpread($E153,Trigger)</f>
@@ -8978,11 +8976,11 @@
       </c>
       <c r="K153" s="11">
         <f>_xll.qlRateHelperEarliestDate($E153,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L153" s="10">
         <f>_xll.qlRateHelperLatestDate($E153,Trigger)</f>
-        <v>46801</v>
+        <v>46818</v>
       </c>
     </row>
     <row r="154" spans="2:12" x14ac:dyDescent="0.2">
@@ -9003,7 +9001,7 @@
       </c>
       <c r="F154" s="13">
         <f>_xll.qlRateHelperQuoteValue($E154,Trigger)</f>
-        <v>2.5740000000000002E-2</v>
+        <v>2.3869999999999999E-2</v>
       </c>
       <c r="G154" s="13">
         <f>_xll.qlSwapRateHelperSpread($E154,Trigger)</f>
@@ -9020,11 +9018,11 @@
       </c>
       <c r="K154" s="11">
         <f>_xll.qlRateHelperEarliestDate($E154,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L154" s="10">
         <f>_xll.qlRateHelperLatestDate($E154,Trigger)</f>
-        <v>47168</v>
+        <v>47183</v>
       </c>
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.2">
@@ -9045,7 +9043,7 @@
       </c>
       <c r="F155" s="13">
         <f>_xll.qlRateHelperQuoteValue($E155,Trigger)</f>
-        <v>2.6185999999999997E-2</v>
+        <v>2.4315E-2</v>
       </c>
       <c r="G155" s="13">
         <f>_xll.qlSwapRateHelperSpread($E155,Trigger)</f>
@@ -9062,11 +9060,11 @@
       </c>
       <c r="K155" s="11">
         <f>_xll.qlRateHelperEarliestDate($E155,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L155" s="10">
         <f>_xll.qlRateHelperLatestDate($E155,Trigger)</f>
-        <v>47532</v>
+        <v>47548</v>
       </c>
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.2">
@@ -9087,7 +9085,7 @@
       </c>
       <c r="F156" s="13">
         <f>_xll.qlRateHelperQuoteValue($E156,Trigger)</f>
-        <v>2.6527000000000002E-2</v>
+        <v>2.4664000000000002E-2</v>
       </c>
       <c r="G156" s="13">
         <f>_xll.qlSwapRateHelperSpread($E156,Trigger)</f>
@@ -9104,11 +9102,11 @@
       </c>
       <c r="K156" s="11">
         <f>_xll.qlRateHelperEarliestDate($E156,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L156" s="10">
         <f>_xll.qlRateHelperLatestDate($E156,Trigger)</f>
-        <v>47897</v>
+        <v>47913</v>
       </c>
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.2">
@@ -9129,7 +9127,7 @@
       </c>
       <c r="F157" s="13">
         <f>_xll.qlRateHelperQuoteValue($E157,Trigger)</f>
-        <v>2.6781000000000003E-2</v>
+        <v>2.4936E-2</v>
       </c>
       <c r="G157" s="13">
         <f>_xll.qlSwapRateHelperSpread($E157,Trigger)</f>
@@ -9146,11 +9144,11 @@
       </c>
       <c r="K157" s="11">
         <f>_xll.qlRateHelperEarliestDate($E157,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L157" s="10">
         <f>_xll.qlRateHelperLatestDate($E157,Trigger)</f>
-        <v>48262</v>
+        <v>48281</v>
       </c>
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.2">
@@ -9171,7 +9169,7 @@
       </c>
       <c r="F158" s="13">
         <f>_xll.qlRateHelperQuoteValue($E158,Trigger)</f>
-        <v>2.6979E-2</v>
+        <v>2.5131999999999998E-2</v>
       </c>
       <c r="G158" s="13">
         <f>_xll.qlSwapRateHelperSpread($E158,Trigger)</f>
@@ -9188,11 +9186,11 @@
       </c>
       <c r="K158" s="11">
         <f>_xll.qlRateHelperEarliestDate($E158,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L158" s="10">
         <f>_xll.qlRateHelperLatestDate($E158,Trigger)</f>
-        <v>48628</v>
+        <v>48645</v>
       </c>
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.2">
@@ -9213,7 +9211,7 @@
       </c>
       <c r="F159" s="13">
         <f>_xll.qlRateHelperQuoteValue($E159,Trigger)</f>
-        <v>2.7120000000000002E-2</v>
+        <v>2.528E-2</v>
       </c>
       <c r="G159" s="13">
         <f>_xll.qlSwapRateHelperSpread($E159,Trigger)</f>
@@ -9230,11 +9228,11 @@
       </c>
       <c r="K159" s="11">
         <f>_xll.qlRateHelperEarliestDate($E159,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L159" s="10">
         <f>_xll.qlRateHelperLatestDate($E159,Trigger)</f>
-        <v>48995</v>
+        <v>49009</v>
       </c>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.2">
@@ -9255,7 +9253,7 @@
       </c>
       <c r="F160" s="13">
         <f>_xll.qlRateHelperQuoteValue($E160,Trigger)</f>
-        <v>2.7243E-2</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="G160" s="13">
         <f>_xll.qlSwapRateHelperSpread($E160,Trigger)</f>
@@ -9272,11 +9270,11 @@
       </c>
       <c r="K160" s="11">
         <f>_xll.qlRateHelperEarliestDate($E160,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L160" s="10">
         <f>_xll.qlRateHelperLatestDate($E160,Trigger)</f>
-        <v>49359</v>
+        <v>49374</v>
       </c>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.2">
@@ -9297,7 +9295,7 @@
       </c>
       <c r="F161" s="13">
         <f>_xll.qlRateHelperQuoteValue($E161,Trigger)</f>
-        <v>2.7318000000000002E-2</v>
+        <v>2.5503000000000001E-2</v>
       </c>
       <c r="G161" s="13">
         <f>_xll.qlSwapRateHelperSpread($E161,Trigger)</f>
@@ -9314,11 +9312,11 @@
       </c>
       <c r="K161" s="11">
         <f>_xll.qlRateHelperEarliestDate($E161,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L161" s="10">
         <f>_xll.qlRateHelperLatestDate($E161,Trigger)</f>
-        <v>49723</v>
+        <v>49740</v>
       </c>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.2">
@@ -9339,7 +9337,7 @@
       </c>
       <c r="F162" s="13">
         <f>_xll.qlRateHelperQuoteValue($E162,Trigger)</f>
-        <v>2.7384000000000002E-2</v>
+        <v>2.5566999999999999E-2</v>
       </c>
       <c r="G162" s="13">
         <f>_xll.qlSwapRateHelperSpread($E162,Trigger)</f>
@@ -9356,11 +9354,11 @@
       </c>
       <c r="K162" s="11">
         <f>_xll.qlRateHelperEarliestDate($E162,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L162" s="10">
         <f>_xll.qlRateHelperLatestDate($E162,Trigger)</f>
-        <v>50089</v>
+        <v>50105</v>
       </c>
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.2">
@@ -9381,7 +9379,7 @@
       </c>
       <c r="F163" s="13">
         <f>_xll.qlRateHelperQuoteValue($E163,Trigger)</f>
-        <v>2.7421999999999998E-2</v>
+        <v>2.5623E-2</v>
       </c>
       <c r="G163" s="13">
         <f>_xll.qlSwapRateHelperSpread($E163,Trigger)</f>
@@ -9398,11 +9396,11 @@
       </c>
       <c r="K163" s="11">
         <f>_xll.qlRateHelperEarliestDate($E163,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L163" s="10">
         <f>_xll.qlRateHelperLatestDate($E163,Trigger)</f>
-        <v>50454</v>
+        <v>50472</v>
       </c>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.2">
@@ -9423,7 +9421,7 @@
       </c>
       <c r="F164" s="13">
         <f>_xll.qlRateHelperQuoteValue($E164,Trigger)</f>
-        <v>2.7440000000000003E-2</v>
+        <v>2.5649999999999999E-2</v>
       </c>
       <c r="G164" s="13">
         <f>_xll.qlSwapRateHelperSpread($E164,Trigger)</f>
@@ -9440,11 +9438,11 @@
       </c>
       <c r="K164" s="11">
         <f>_xll.qlRateHelperEarliestDate($E164,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L164" s="10">
         <f>_xll.qlRateHelperLatestDate($E164,Trigger)</f>
-        <v>50819</v>
+        <v>50836</v>
       </c>
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.2">
@@ -9465,7 +9463,7 @@
       </c>
       <c r="F165" s="13">
         <f>_xll.qlRateHelperQuoteValue($E165,Trigger)</f>
-        <v>2.7439000000000002E-2</v>
+        <v>2.5669000000000001E-2</v>
       </c>
       <c r="G165" s="13">
         <f>_xll.qlSwapRateHelperSpread($E165,Trigger)</f>
@@ -9482,11 +9480,11 @@
       </c>
       <c r="K165" s="11">
         <f>_xll.qlRateHelperEarliestDate($E165,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L165" s="10">
         <f>_xll.qlRateHelperLatestDate($E165,Trigger)</f>
-        <v>51186</v>
+        <v>51201</v>
       </c>
     </row>
     <row r="166" spans="2:12" x14ac:dyDescent="0.2">
@@ -9507,7 +9505,7 @@
       </c>
       <c r="F166" s="13">
         <f>_xll.qlRateHelperQuoteValue($E166,Trigger)</f>
-        <v>2.7438999999999998E-2</v>
+        <v>2.5668E-2</v>
       </c>
       <c r="G166" s="13">
         <f>_xll.qlSwapRateHelperSpread($E166,Trigger)</f>
@@ -9524,11 +9522,11 @@
       </c>
       <c r="K166" s="11">
         <f>_xll.qlRateHelperEarliestDate($E166,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L166" s="10">
         <f>_xll.qlRateHelperLatestDate($E166,Trigger)</f>
-        <v>51550</v>
+        <v>51566</v>
       </c>
     </row>
     <row r="167" spans="2:12" x14ac:dyDescent="0.2">
@@ -9549,7 +9547,7 @@
       </c>
       <c r="F167" s="13">
         <f>_xll.qlRateHelperQuoteValue($E167,Trigger)</f>
-        <v>2.7419000000000002E-2</v>
+        <v>2.5668E-2</v>
       </c>
       <c r="G167" s="13">
         <f>_xll.qlSwapRateHelperSpread($E167,Trigger)</f>
@@ -9566,11 +9564,11 @@
       </c>
       <c r="K167" s="11">
         <f>_xll.qlRateHelperEarliestDate($E167,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L167" s="10">
         <f>_xll.qlRateHelperLatestDate($E167,Trigger)</f>
-        <v>51915</v>
+        <v>51931</v>
       </c>
     </row>
     <row r="168" spans="2:12" x14ac:dyDescent="0.2">
@@ -9591,7 +9589,7 @@
       </c>
       <c r="F168" s="13">
         <f>_xll.qlRateHelperQuoteValue($E168,Trigger)</f>
-        <v>2.7399000000000003E-2</v>
+        <v>2.5659000000000001E-2</v>
       </c>
       <c r="G168" s="13">
         <f>_xll.qlSwapRateHelperSpread($E168,Trigger)</f>
@@ -9608,11 +9606,11 @@
       </c>
       <c r="K168" s="11">
         <f>_xll.qlRateHelperEarliestDate($E168,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L168" s="10">
         <f>_xll.qlRateHelperLatestDate($E168,Trigger)</f>
-        <v>52280</v>
+        <v>52296</v>
       </c>
     </row>
     <row r="169" spans="2:12" x14ac:dyDescent="0.2">
@@ -9633,7 +9631,7 @@
       </c>
       <c r="F169" s="13">
         <f>_xll.qlRateHelperQuoteValue($E169,Trigger)</f>
-        <v>2.7390000000000001E-2</v>
+        <v>2.5649999999999999E-2</v>
       </c>
       <c r="G169" s="13">
         <f>_xll.qlSwapRateHelperSpread($E169,Trigger)</f>
@@ -9650,11 +9648,11 @@
       </c>
       <c r="K169" s="11">
         <f>_xll.qlRateHelperEarliestDate($E169,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L169" s="10">
         <f>_xll.qlRateHelperLatestDate($E169,Trigger)</f>
-        <v>52645</v>
+        <v>52663</v>
       </c>
     </row>
     <row r="170" spans="2:12" x14ac:dyDescent="0.2">
@@ -9675,7 +9673,7 @@
       </c>
       <c r="F170" s="13">
         <f>_xll.qlRateHelperQuoteValue($E170,Trigger)</f>
-        <v>2.7470000000000001E-2</v>
+        <v>2.5730000000000003E-2</v>
       </c>
       <c r="G170" s="13">
         <f>_xll.qlSwapRateHelperSpread($E170,Trigger)</f>
@@ -9692,11 +9690,11 @@
       </c>
       <c r="K170" s="11">
         <f>_xll.qlRateHelperEarliestDate($E170,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L170" s="10">
         <f>_xll.qlRateHelperLatestDate($E170,Trigger)</f>
-        <v>54472</v>
+        <v>54490</v>
       </c>
     </row>
     <row r="171" spans="2:12" x14ac:dyDescent="0.2">
@@ -9717,7 +9715,7 @@
       </c>
       <c r="F171" s="13">
         <f>_xll.qlRateHelperQuoteValue($E171,Trigger)</f>
-        <v>2.7630000000000002E-2</v>
+        <v>2.5860000000000001E-2</v>
       </c>
       <c r="G171" s="13">
         <f>_xll.qlSwapRateHelperSpread($E171,Trigger)</f>
@@ -9734,11 +9732,11 @@
       </c>
       <c r="K171" s="11">
         <f>_xll.qlRateHelperEarliestDate($E171,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L171" s="10">
         <f>_xll.qlRateHelperLatestDate($E171,Trigger)</f>
-        <v>56298</v>
+        <v>56314</v>
       </c>
     </row>
     <row r="172" spans="2:12" x14ac:dyDescent="0.2">
@@ -9759,7 +9757,7 @@
       </c>
       <c r="F172" s="13">
         <f>_xll.qlRateHelperQuoteValue($E172,Trigger)</f>
-        <v>2.7819999999999998E-2</v>
+        <v>2.6000000000000002E-2</v>
       </c>
       <c r="G172" s="13">
         <f>_xll.qlSwapRateHelperSpread($E172,Trigger)</f>
@@ -9776,11 +9774,11 @@
       </c>
       <c r="K172" s="11">
         <f>_xll.qlRateHelperEarliestDate($E172,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L172" s="10">
         <f>_xll.qlRateHelperLatestDate($E172,Trigger)</f>
-        <v>59950</v>
+        <v>59967</v>
       </c>
     </row>
     <row r="173" spans="2:12" x14ac:dyDescent="0.2">
@@ -9801,7 +9799,7 @@
       </c>
       <c r="F173" s="6">
         <f>_xll.qlRateHelperQuoteValue($E173,Trigger)</f>
-        <v>2.7950000000000003E-2</v>
+        <v>2.613E-2</v>
       </c>
       <c r="G173" s="6">
         <f>_xll.qlSwapRateHelperSpread($E173,Trigger)</f>
@@ -9818,11 +9816,11 @@
       </c>
       <c r="K173" s="4">
         <f>_xll.qlRateHelperEarliestDate($E173,Trigger)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="L173" s="3">
         <f>_xll.qlRateHelperLatestDate($E173,Trigger)</f>
-        <v>63604</v>
+        <v>63619</v>
       </c>
     </row>
   </sheetData>
@@ -9841,8 +9839,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -9862,10 +9860,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="204" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="193"/>
+      <c r="B1" s="205"/>
       <c r="D1" s="53" t="s">
         <v>87</v>
       </c>
@@ -9905,14 +9903,14 @@
       </c>
       <c r="G2" s="40">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H2" s="39">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41716</v>
+        <v>41736</v>
       </c>
       <c r="I2" s="34">
-        <v>0.99954233177833063</v>
+        <v>0.99947698479915448</v>
       </c>
       <c r="K2" s="187" t="s">
         <v>117</v>
@@ -9941,14 +9939,14 @@
       </c>
       <c r="G3" s="40">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H3" s="39">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41778</v>
+        <v>41796</v>
       </c>
       <c r="I3" s="34">
-        <v>0.99853838943246809</v>
+        <v>0.99850595772447803</v>
       </c>
       <c r="K3" s="187" t="s">
         <v>118</v>
@@ -9977,14 +9975,14 @@
       </c>
       <c r="G4" s="40">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H4" s="39">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41869</v>
+        <v>41890</v>
       </c>
       <c r="I4" s="34">
-        <v>0.99711786128943314</v>
+        <v>0.9970384799855907</v>
       </c>
       <c r="K4" s="187" t="s">
         <v>119</v>
@@ -10013,14 +10011,14 @@
       </c>
       <c r="G5" s="40">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H5" s="39">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41961</v>
+        <v>41981</v>
       </c>
       <c r="I5" s="34">
-        <v>0.99569234450739386</v>
+        <v>0.995629504523456</v>
       </c>
       <c r="K5" s="187" t="s">
         <v>120</v>
@@ -10050,11 +10048,11 @@
       </c>
       <c r="G6" s="40">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H6" s="39">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>42053</v>
+        <v>42069</v>
       </c>
       <c r="I6" s="34">
         <v>0.99425404019271957</v>
@@ -10069,7 +10067,7 @@
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_RateHelpersSelected#0002</v>
+        <v>EUR_YC1YRH_RateHelpersSelected#0001</v>
       </c>
       <c r="B7" s="43" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -10088,14 +10086,14 @@
       </c>
       <c r="G7" s="40">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41778</v>
+        <v>41796</v>
       </c>
       <c r="H7" s="39">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>42143</v>
+        <v>42163</v>
       </c>
       <c r="I7" s="34">
-        <v>0.99281083614069399</v>
+        <v>0.99274738861523393</v>
       </c>
       <c r="K7" s="187" t="s">
         <v>122</v>
@@ -10118,14 +10116,14 @@
       </c>
       <c r="G8" s="40">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41869</v>
+        <v>41890</v>
       </c>
       <c r="H8" s="39">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>42234</v>
+        <v>42255</v>
       </c>
       <c r="I8" s="34">
-        <v>0.99124956747849813</v>
+        <v>0.99117065335394594</v>
       </c>
       <c r="K8" s="187" t="s">
         <v>123</v>
@@ -10148,14 +10146,14 @@
       </c>
       <c r="G9" s="40">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41961</v>
+        <v>41981</v>
       </c>
       <c r="H9" s="39">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42326</v>
+        <v>42346</v>
       </c>
       <c r="I9" s="34">
-        <v>0.98950032632669438</v>
+        <v>0.98943787713245912</v>
       </c>
       <c r="K9" s="187" t="s">
         <v>124</v>
@@ -10170,7 +10168,7 @@
       </c>
       <c r="E10" s="41">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>6.7400000000000003E-3</v>
+        <v>6.3899999999999998E-3</v>
       </c>
       <c r="F10" s="41" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -10178,14 +10176,14 @@
       </c>
       <c r="G10" s="40">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>42053</v>
+        <v>42069</v>
       </c>
       <c r="H10" s="39">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42418</v>
+        <v>42436</v>
       </c>
       <c r="I10" s="34">
-        <v>0.9875058095204936</v>
+        <v>0.98781913936415011</v>
       </c>
       <c r="K10" s="187" t="s">
         <v>125</v>
@@ -10208,14 +10206,14 @@
       </c>
       <c r="G11" s="40">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>42142</v>
+        <v>42163</v>
       </c>
       <c r="H11" s="39">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42508</v>
+        <v>42529</v>
       </c>
       <c r="I11" s="34">
-        <v>0.98531129822262042</v>
+        <v>0.98523198973592874</v>
       </c>
       <c r="K11" s="187" t="s">
         <v>126</v>
@@ -10238,14 +10236,14 @@
       </c>
       <c r="G12" s="40">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>42234</v>
+        <v>42254</v>
       </c>
       <c r="H12" s="39">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42600</v>
+        <v>42620</v>
       </c>
       <c r="I12" s="34">
-        <v>0.98272125040845359</v>
+        <v>0.98266154729473021</v>
       </c>
       <c r="K12" s="187" t="s">
         <v>127</v>
@@ -10260,7 +10258,7 @@
       </c>
       <c r="E13" s="41">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>7.9900000000000006E-3</v>
+        <v>7.4800000000000005E-3</v>
       </c>
       <c r="F13" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -10268,14 +10266,14 @@
       </c>
       <c r="G13" s="40">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H13" s="39">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42786</v>
+        <v>42800</v>
       </c>
       <c r="I13" s="34">
-        <v>0.97632159145442765</v>
+        <v>0.97767938874527982</v>
       </c>
       <c r="K13" s="187" t="s">
         <v>128</v>
@@ -10290,7 +10288,7 @@
       </c>
       <c r="E14" s="41">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>1.027E-2</v>
+        <v>9.4500000000000001E-3</v>
       </c>
       <c r="F14" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -10298,14 +10296,14 @@
       </c>
       <c r="G14" s="40">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H14" s="39">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>43150</v>
+        <v>43165</v>
       </c>
       <c r="I14" s="34">
-        <v>0.95973569259205038</v>
+        <v>0.96275062727104432</v>
       </c>
       <c r="K14" s="187" t="s">
         <v>129</v>
@@ -10320,7 +10318,7 @@
       </c>
       <c r="E15" s="41">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>1.2610000000000001E-2</v>
+        <v>1.149E-2</v>
       </c>
       <c r="F15" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -10328,14 +10326,14 @@
       </c>
       <c r="G15" s="40">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H15" s="39">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>43514</v>
+        <v>43530</v>
       </c>
       <c r="I15" s="34">
-        <v>0.93875670708534265</v>
+        <v>0.9439032153491268</v>
       </c>
       <c r="K15" s="187" t="s">
         <v>130</v>
@@ -10350,7 +10348,7 @@
       </c>
       <c r="E16" s="41">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>1.4789999999999999E-2</v>
+        <v>1.345E-2</v>
       </c>
       <c r="F16" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -10358,14 +10356,14 @@
       </c>
       <c r="G16" s="40">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H16" s="39">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>43879</v>
+        <v>43896</v>
       </c>
       <c r="I16" s="34">
-        <v>0.91464150040818726</v>
+        <v>0.92196457997770997</v>
       </c>
       <c r="K16" s="187" t="s">
         <v>131</v>
@@ -10380,7 +10378,7 @@
       </c>
       <c r="E17" s="41">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>1.677E-2</v>
+        <v>1.5269999999999999E-2</v>
       </c>
       <c r="F17" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -10388,14 +10386,14 @@
       </c>
       <c r="G17" s="40">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H17" s="39">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>44245</v>
+        <v>44263</v>
       </c>
       <c r="I17" s="34">
-        <v>0.88831711813212222</v>
+        <v>0.89764648139807868</v>
       </c>
       <c r="K17" s="187" t="s">
         <v>132</v>
@@ -10410,7 +10408,7 @@
       </c>
       <c r="E18" s="41">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>1.8540000000000001E-2</v>
+        <v>1.6910000000000001E-2</v>
       </c>
       <c r="F18" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -10418,14 +10416,14 @@
       </c>
       <c r="G18" s="40">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H18" s="39">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>44610</v>
+        <v>44627</v>
       </c>
       <c r="I18" s="34">
-        <v>0.86057442951446128</v>
+        <v>0.87196914802988867</v>
       </c>
       <c r="K18" s="187" t="s">
         <v>133</v>
@@ -10440,7 +10438,7 @@
       </c>
       <c r="E19" s="41">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>2.0110000000000003E-2</v>
+        <v>1.8380000000000001E-2</v>
       </c>
       <c r="F19" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -10448,14 +10446,14 @@
       </c>
       <c r="G19" s="40">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H19" s="39">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>44977</v>
+        <v>44991</v>
       </c>
       <c r="I19" s="34">
-        <v>0.83194427941853755</v>
+        <v>0.84536052986764443</v>
       </c>
       <c r="K19" s="187" t="s">
         <v>134</v>
@@ -10470,7 +10468,7 @@
       </c>
       <c r="E20" s="41">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>2.147E-2</v>
+        <v>1.9700000000000002E-2</v>
       </c>
       <c r="F20" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -10478,14 +10476,14 @@
       </c>
       <c r="G20" s="40">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H20" s="39">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>45341</v>
+        <v>45357</v>
       </c>
       <c r="I20" s="34">
-        <v>0.80337837827113301</v>
+        <v>0.81815022907220014</v>
       </c>
       <c r="K20" s="187" t="s">
         <v>135</v>
@@ -10500,7 +10498,7 @@
       </c>
       <c r="E21" s="41">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>2.3640000000000001E-2</v>
+        <v>2.1789999999999997E-2</v>
       </c>
       <c r="F21" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -10508,14 +10506,14 @@
       </c>
       <c r="G21" s="40">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H21" s="39">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>46071</v>
+        <v>46087</v>
       </c>
       <c r="I21" s="34">
-        <v>0.74756039277880337</v>
+        <v>0.76496611703926243</v>
       </c>
       <c r="K21" s="187" t="s">
         <v>136</v>
@@ -10530,7 +10528,7 @@
       </c>
       <c r="E22" s="41">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>2.5740000000000002E-2</v>
+        <v>2.3869999999999999E-2</v>
       </c>
       <c r="F22" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -10538,14 +10536,14 @@
       </c>
       <c r="G22" s="40">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H22" s="39">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>47168</v>
+        <v>47183</v>
       </c>
       <c r="I22" s="34">
-        <v>0.67134728871161886</v>
+        <v>0.69133742715415136</v>
       </c>
       <c r="K22" s="187" t="s">
         <v>137</v>
@@ -10560,7 +10558,7 @@
       </c>
       <c r="E23" s="41">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>2.7120000000000002E-2</v>
+        <v>2.528E-2</v>
       </c>
       <c r="F23" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -10568,14 +10566,14 @@
       </c>
       <c r="G23" s="40">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H23" s="39">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>48995</v>
+        <v>49009</v>
       </c>
       <c r="I23" s="34">
-        <v>0.57111895971306614</v>
+        <v>0.59343592249700805</v>
       </c>
       <c r="K23" s="187" t="s">
         <v>138</v>
@@ -10590,7 +10588,7 @@
       </c>
       <c r="E24" s="41">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>2.7440000000000003E-2</v>
+        <v>2.5649999999999999E-2</v>
       </c>
       <c r="F24" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -10598,14 +10596,14 @@
       </c>
       <c r="G24" s="40">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H24" s="39">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>50819</v>
+        <v>50836</v>
       </c>
       <c r="I24" s="34">
-        <v>0.49431460686077139</v>
+        <v>0.51738052442685156</v>
       </c>
       <c r="K24" s="187" t="s">
         <v>139</v>
@@ -10620,7 +10618,7 @@
       </c>
       <c r="E25" s="41">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>2.7390000000000001E-2</v>
+        <v>2.5649999999999999E-2</v>
       </c>
       <c r="F25" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -10628,14 +10626,14 @@
       </c>
       <c r="G25" s="40">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H25" s="39">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>52645</v>
+        <v>52663</v>
       </c>
       <c r="I25" s="34">
-        <v>0.43270532317582572</v>
+        <v>0.45585545726629456</v>
       </c>
       <c r="K25" s="187" t="s">
         <v>140</v>
@@ -10650,7 +10648,7 @@
       </c>
       <c r="E26" s="41">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>2.7470000000000001E-2</v>
+        <v>2.5730000000000003E-2</v>
       </c>
       <c r="F26" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -10658,14 +10656,14 @@
       </c>
       <c r="G26" s="40">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H26" s="39">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>54472</v>
+        <v>54490</v>
       </c>
       <c r="I26" s="34">
-        <v>0.37630612436793942</v>
+        <v>0.39984856952769215</v>
       </c>
       <c r="K26" s="187" t="s">
         <v>141</v>
@@ -10680,7 +10678,7 @@
       </c>
       <c r="E27" s="41">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>2.7630000000000002E-2</v>
+        <v>2.5860000000000001E-2</v>
       </c>
       <c r="F27" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -10688,14 +10686,14 @@
       </c>
       <c r="G27" s="40">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H27" s="39">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>56298</v>
+        <v>56314</v>
       </c>
       <c r="I27" s="34">
-        <v>0.32501075414272979</v>
+        <v>0.34916867556882936</v>
       </c>
       <c r="K27" s="187" t="s">
         <v>142</v>
@@ -10710,7 +10708,7 @@
       </c>
       <c r="E28" s="41">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.7819999999999998E-2</v>
+        <v>2.6000000000000002E-2</v>
       </c>
       <c r="F28" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -10718,14 +10716,14 @@
       </c>
       <c r="G28" s="40">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H28" s="39">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>59950</v>
+        <v>59967</v>
       </c>
       <c r="I28" s="34">
-        <v>0.24305954745722594</v>
+        <v>0.26708061740853006</v>
       </c>
       <c r="K28" s="187" t="s">
         <v>143</v>
@@ -10740,7 +10738,7 @@
       </c>
       <c r="E29" s="41">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.7950000000000003E-2</v>
+        <v>2.613E-2</v>
       </c>
       <c r="F29" s="41">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -10748,14 +10746,14 @@
       </c>
       <c r="G29" s="40">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>41688</v>
+        <v>41704</v>
       </c>
       <c r="H29" s="39">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>63604</v>
+        <v>63619</v>
       </c>
       <c r="I29" s="34">
-        <v>0.18144476455568445</v>
+        <v>0.20316032572374745</v>
       </c>
       <c r="K29" s="187" t="s">
         <v>144</v>
@@ -13130,7 +13128,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="108" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" s="107"/>
       <c r="C1" s="107"/>
@@ -13184,7 +13182,7 @@
       </c>
       <c r="F3" s="98" t="str">
         <f>_xll.qlDepositRateHelper2(E3,D3,"1d",2,"target","following",FALSE,"act/360",Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_SND#0003</v>
+        <v>EUR_YC1YRH_SND#0001</v>
       </c>
       <c r="G3" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -13211,7 +13209,7 @@
       </c>
       <c r="F4" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_SWD#0003</v>
+        <v>EUR_YC1YRH_SWD#0001</v>
       </c>
       <c r="G4" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -13238,7 +13236,7 @@
       </c>
       <c r="F5" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_2WD#0003</v>
+        <v>EUR_YC1YRH_2WD#0001</v>
       </c>
       <c r="G5" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -13265,7 +13263,7 @@
       </c>
       <c r="F6" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_3WD#0003</v>
+        <v>EUR_YC1YRH_3WD#0001</v>
       </c>
       <c r="G6" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -13292,7 +13290,7 @@
       </c>
       <c r="F7" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_1MD#0003</v>
+        <v>EUR_YC1YRH_1MD#0001</v>
       </c>
       <c r="G7" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -13319,7 +13317,7 @@
       </c>
       <c r="F8" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_2MD#0003</v>
+        <v>EUR_YC1YRH_2MD#0001</v>
       </c>
       <c r="G8" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -13346,7 +13344,7 @@
       </c>
       <c r="F9" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_3MD#0003</v>
+        <v>EUR_YC1YRH_3MD#0001</v>
       </c>
       <c r="G9" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -13373,7 +13371,7 @@
       </c>
       <c r="F10" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E10,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_4MD#0003</v>
+        <v>EUR_YC1YRH_4MD#0001</v>
       </c>
       <c r="G10" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -13400,7 +13398,7 @@
       </c>
       <c r="F11" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E11,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_5MD#0003</v>
+        <v>EUR_YC1YRH_5MD#0001</v>
       </c>
       <c r="G11" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -13427,7 +13425,7 @@
       </c>
       <c r="F12" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E12,D12,C12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_6MD#0003</v>
+        <v>EUR_YC1YRH_6MD#0001</v>
       </c>
       <c r="G12" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F12)</f>
@@ -13454,7 +13452,7 @@
       </c>
       <c r="F13" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E13,D13,C13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_7MD#0003</v>
+        <v>EUR_YC1YRH_7MD#0001</v>
       </c>
       <c r="G13" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F13)</f>
@@ -13481,7 +13479,7 @@
       </c>
       <c r="F14" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E14,D14,C14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_8MD#0003</v>
+        <v>EUR_YC1YRH_8MD#0001</v>
       </c>
       <c r="G14" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F14)</f>
@@ -13508,7 +13506,7 @@
       </c>
       <c r="F15" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E15,D15,C15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_9MD#0003</v>
+        <v>EUR_YC1YRH_9MD#0001</v>
       </c>
       <c r="G15" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F15)</f>
@@ -13535,7 +13533,7 @@
       </c>
       <c r="F16" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E16,D16,C16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_10MD#0003</v>
+        <v>EUR_YC1YRH_10MD#0001</v>
       </c>
       <c r="G16" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F16)</f>
@@ -13562,7 +13560,7 @@
       </c>
       <c r="F17" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E17,D17,C17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_11MD#0003</v>
+        <v>EUR_YC1YRH_11MD#0001</v>
       </c>
       <c r="G17" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F17)</f>
@@ -13589,7 +13587,7 @@
       </c>
       <c r="F18" s="92" t="str">
         <f>_xll.qlDepositRateHelper(E18,D18,C18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_1YD#0003</v>
+        <v>EUR_YC1YRH_1YD#0001</v>
       </c>
       <c r="G18" s="91" t="str">
         <f>_xll.ohRangeRetrieveError(F18)</f>
@@ -13638,7 +13636,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="186" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B1" s="161"/>
       <c r="C1" s="162"/>
@@ -13715,7 +13713,7 @@
       </c>
       <c r="I3" s="139" t="str">
         <f>_xll.qlFraRateHelper(H3,G3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_T12F1#0003</v>
+        <v>EUR_YC1YRH_T12F1#0001</v>
       </c>
       <c r="J3" s="149" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -13752,7 +13750,7 @@
       </c>
       <c r="I4" s="130" t="str">
         <f>_xll.qlFraRateHelper(H4,G4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_TOM12F1#0003</v>
+        <v>EUR_YC1YRH_TOM12F1#0001</v>
       </c>
       <c r="J4" s="148" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -13790,7 +13788,7 @@
       </c>
       <c r="I5" s="134" t="str">
         <f>_xll.qlFraRateHelper(H5,G5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_1x13F#0003</v>
+        <v>EUR_YC1YRH_1x13F#0001</v>
       </c>
       <c r="J5" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -13828,7 +13826,7 @@
       </c>
       <c r="I6" s="134" t="str">
         <f>_xll.qlFraRateHelper(H6,G6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_2x14F#0003</v>
+        <v>EUR_YC1YRH_2x14F#0001</v>
       </c>
       <c r="J6" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -13866,7 +13864,7 @@
       </c>
       <c r="I7" s="134" t="str">
         <f>_xll.qlFraRateHelper(H7,G7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_3x15F#0003</v>
+        <v>EUR_YC1YRH_3x15F#0001</v>
       </c>
       <c r="J7" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -13904,7 +13902,7 @@
       </c>
       <c r="I8" s="134" t="str">
         <f>_xll.qlFraRateHelper(H8,G8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_4x16F#0003</v>
+        <v>EUR_YC1YRH_4x16F#0001</v>
       </c>
       <c r="J8" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -13942,7 +13940,7 @@
       </c>
       <c r="I9" s="134" t="str">
         <f>_xll.qlFraRateHelper(H9,G9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_5x17F#0003</v>
+        <v>EUR_YC1YRH_5x17F#0001</v>
       </c>
       <c r="J9" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -13980,7 +13978,7 @@
       </c>
       <c r="I10" s="134" t="str">
         <f>_xll.qlFraRateHelper(H10,G10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_6x18F#0003</v>
+        <v>EUR_YC1YRH_6x18F#0001</v>
       </c>
       <c r="J10" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -14018,7 +14016,7 @@
       </c>
       <c r="I11" s="134" t="str">
         <f>_xll.qlFraRateHelper(H11,G11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_7x19F#0003</v>
+        <v>EUR_YC1YRH_7x19F#0001</v>
       </c>
       <c r="J11" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -14056,7 +14054,7 @@
       </c>
       <c r="I12" s="134" t="str">
         <f>_xll.qlFraRateHelper(H12,G12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_8x20F#0003</v>
+        <v>EUR_YC1YRH_8x20F#0001</v>
       </c>
       <c r="J12" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -14094,7 +14092,7 @@
       </c>
       <c r="I13" s="134" t="str">
         <f>_xll.qlFraRateHelper(H13,G13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_9x21F#0003</v>
+        <v>EUR_YC1YRH_9x21F#0001</v>
       </c>
       <c r="J13" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -14132,7 +14130,7 @@
       </c>
       <c r="I14" s="134" t="str">
         <f>_xll.qlFraRateHelper(H14,G14,B14,E14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_10x22F#0003</v>
+        <v>EUR_YC1YRH_10x22F#0001</v>
       </c>
       <c r="J14" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -14170,7 +14168,7 @@
       </c>
       <c r="I15" s="134" t="str">
         <f>_xll.qlFraRateHelper(H15,G15,B15,E15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_11x23F#0003</v>
+        <v>EUR_YC1YRH_11x23F#0001</v>
       </c>
       <c r="J15" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I15)</f>
@@ -14208,7 +14206,7 @@
       </c>
       <c r="I16" s="144" t="str">
         <f>_xll.qlFraRateHelper(H16,G16,B16,E16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_12x24F#0003</v>
+        <v>EUR_YC1YRH_12x24F#0001</v>
       </c>
       <c r="J16" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -14246,7 +14244,7 @@
       </c>
       <c r="I17" s="139" t="str">
         <f>_xll.qlFraRateHelper(H17,G17,B17,E17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_13x25F#0003</v>
+        <v>EUR_YC1YRH_13x25F#0001</v>
       </c>
       <c r="J17" s="138" t="str">
         <f>_xll.ohRangeRetrieveError(I17)</f>
@@ -14284,7 +14282,7 @@
       </c>
       <c r="I18" s="134" t="str">
         <f>_xll.qlFraRateHelper(H18,G18,B18,E18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_14x26F#0003</v>
+        <v>EUR_YC1YRH_14x26F#0001</v>
       </c>
       <c r="J18" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I18)</f>
@@ -14322,7 +14320,7 @@
       </c>
       <c r="I19" s="134" t="str">
         <f>_xll.qlFraRateHelper(H19,G19,B19,E19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_15x27F#0003</v>
+        <v>EUR_YC1YRH_15x27F#0001</v>
       </c>
       <c r="J19" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I19)</f>
@@ -14360,7 +14358,7 @@
       </c>
       <c r="I20" s="134" t="str">
         <f>_xll.qlFraRateHelper(H20,G20,B20,E20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_16x28F#0003</v>
+        <v>EUR_YC1YRH_16x28F#0001</v>
       </c>
       <c r="J20" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I20)</f>
@@ -14398,7 +14396,7 @@
       </c>
       <c r="I21" s="134" t="str">
         <f>_xll.qlFraRateHelper(H21,G21,B21,E21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_17x29F#0003</v>
+        <v>EUR_YC1YRH_17x29F#0001</v>
       </c>
       <c r="J21" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I21)</f>
@@ -14436,7 +14434,7 @@
       </c>
       <c r="I22" s="134" t="str">
         <f>_xll.qlFraRateHelper(H22,G22,B22,E22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_18x30F#0003</v>
+        <v>EUR_YC1YRH_18x30F#0001</v>
       </c>
       <c r="J22" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -14474,7 +14472,7 @@
       </c>
       <c r="I23" s="134" t="str">
         <f>_xll.qlFraRateHelper(H23,G23,B23,E23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_19x31F#0003</v>
+        <v>EUR_YC1YRH_19x31F#0001</v>
       </c>
       <c r="J23" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I23)</f>
@@ -14512,7 +14510,7 @@
       </c>
       <c r="I24" s="134" t="str">
         <f>_xll.qlFraRateHelper(H24,G24,B24,E24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_20x32F#0003</v>
+        <v>EUR_YC1YRH_20x32F#0001</v>
       </c>
       <c r="J24" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I24)</f>
@@ -14550,7 +14548,7 @@
       </c>
       <c r="I25" s="134" t="str">
         <f>_xll.qlFraRateHelper(H25,G25,B25,E25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_21x33F#0003</v>
+        <v>EUR_YC1YRH_21x33F#0001</v>
       </c>
       <c r="J25" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I25)</f>
@@ -14588,7 +14586,7 @@
       </c>
       <c r="I26" s="134" t="str">
         <f>_xll.qlFraRateHelper(H26,G26,B26,E26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_22x34F#0003</v>
+        <v>EUR_YC1YRH_22x34F#0001</v>
       </c>
       <c r="J26" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I26)</f>
@@ -14626,7 +14624,7 @@
       </c>
       <c r="I27" s="130" t="str">
         <f>_xll.qlFraRateHelper(H27,G27,B27,E27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_23x35F#0003</v>
+        <v>EUR_YC1YRH_23x35F#0001</v>
       </c>
       <c r="J27" s="129" t="str">
         <f>_xll.ohRangeRetrieveError(I27)</f>
@@ -14664,7 +14662,7 @@
       </c>
       <c r="I28" s="139" t="str">
         <f>_xll.qlFraRateHelper(H28,G28,B28,E28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_25x37F#0003</v>
+        <v>EUR_YC1YRH_25x37F#0001</v>
       </c>
       <c r="J28" s="138" t="str">
         <f>_xll.ohRangeRetrieveError(I28)</f>
@@ -14702,7 +14700,7 @@
       </c>
       <c r="I29" s="134" t="str">
         <f>_xll.qlFraRateHelper(H29,G29,B29,E29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_26x38F#0003</v>
+        <v>EUR_YC1YRH_26x38F#0001</v>
       </c>
       <c r="J29" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I29)</f>
@@ -14740,7 +14738,7 @@
       </c>
       <c r="I30" s="134" t="str">
         <f>_xll.qlFraRateHelper(H30,G30,B30,E30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_27x39F#0003</v>
+        <v>EUR_YC1YRH_27x39F#0001</v>
       </c>
       <c r="J30" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I30)</f>
@@ -14778,7 +14776,7 @@
       </c>
       <c r="I31" s="134" t="str">
         <f>_xll.qlFraRateHelper(H31,G31,B31,E31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_28x40F#0003</v>
+        <v>EUR_YC1YRH_28x40F#0001</v>
       </c>
       <c r="J31" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I31)</f>
@@ -14816,7 +14814,7 @@
       </c>
       <c r="I32" s="134" t="str">
         <f>_xll.qlFraRateHelper(H32,G32,B32,E32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_29x41F#0003</v>
+        <v>EUR_YC1YRH_29x41F#0001</v>
       </c>
       <c r="J32" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I32)</f>
@@ -14854,7 +14852,7 @@
       </c>
       <c r="I33" s="134" t="str">
         <f>_xll.qlFraRateHelper(H33,G33,B33,E33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_30x42F#0003</v>
+        <v>EUR_YC1YRH_30x42F#0001</v>
       </c>
       <c r="J33" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I33)</f>
@@ -14892,7 +14890,7 @@
       </c>
       <c r="I34" s="134" t="str">
         <f>_xll.qlFraRateHelper(H34,G34,B34,E34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_31x43F#0003</v>
+        <v>EUR_YC1YRH_31x43F#0001</v>
       </c>
       <c r="J34" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I34)</f>
@@ -14930,7 +14928,7 @@
       </c>
       <c r="I35" s="134" t="str">
         <f>_xll.qlFraRateHelper(H35,G35,B35,E35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_32x44F#0003</v>
+        <v>EUR_YC1YRH_32x44F#0001</v>
       </c>
       <c r="J35" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I35)</f>
@@ -14968,7 +14966,7 @@
       </c>
       <c r="I36" s="134" t="str">
         <f>_xll.qlFraRateHelper(H36,G36,B36,E36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_33x45F#0003</v>
+        <v>EUR_YC1YRH_33x45F#0001</v>
       </c>
       <c r="J36" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I36)</f>
@@ -15006,7 +15004,7 @@
       </c>
       <c r="I37" s="134" t="str">
         <f>_xll.qlFraRateHelper(H37,G37,B37,E37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_34x46F#0003</v>
+        <v>EUR_YC1YRH_34x46F#0001</v>
       </c>
       <c r="J37" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I37)</f>
@@ -15044,7 +15042,7 @@
       </c>
       <c r="I38" s="130" t="str">
         <f>_xll.qlFraRateHelper(H38,G38,B38,E38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_35x47F#0003</v>
+        <v>EUR_YC1YRH_35x47F#0001</v>
       </c>
       <c r="J38" s="129" t="str">
         <f>_xll.ohRangeRetrieveError(I38)</f>
@@ -15082,7 +15080,7 @@
       </c>
       <c r="I39" s="134" t="str">
         <f>_xll.qlFraRateHelper(H39,G39,B39,E39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_37x49F#0003</v>
+        <v>EUR_YC1YRH_37x49F#0001</v>
       </c>
       <c r="J39" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I39)</f>
@@ -15120,7 +15118,7 @@
       </c>
       <c r="I40" s="134" t="str">
         <f>_xll.qlFraRateHelper(H40,G40,B40,E40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_38x50F#0003</v>
+        <v>EUR_YC1YRH_38x50F#0001</v>
       </c>
       <c r="J40" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I40)</f>
@@ -15158,7 +15156,7 @@
       </c>
       <c r="I41" s="134" t="str">
         <f>_xll.qlFraRateHelper(H41,G41,B41,E41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_39x51F#0003</v>
+        <v>EUR_YC1YRH_39x51F#0001</v>
       </c>
       <c r="J41" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I41)</f>
@@ -15196,7 +15194,7 @@
       </c>
       <c r="I42" s="134" t="str">
         <f>_xll.qlFraRateHelper(H42,G42,B42,E42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_40x52F#0003</v>
+        <v>EUR_YC1YRH_40x52F#0001</v>
       </c>
       <c r="J42" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I42)</f>
@@ -15234,7 +15232,7 @@
       </c>
       <c r="I43" s="134" t="str">
         <f>_xll.qlFraRateHelper(H43,G43,B43,E43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_41x53F#0003</v>
+        <v>EUR_YC1YRH_41x53F#0001</v>
       </c>
       <c r="J43" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I43)</f>
@@ -15272,7 +15270,7 @@
       </c>
       <c r="I44" s="134" t="str">
         <f>_xll.qlFraRateHelper(H44,G44,B44,E44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_42x54F#0003</v>
+        <v>EUR_YC1YRH_42x54F#0001</v>
       </c>
       <c r="J44" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I44)</f>
@@ -15310,7 +15308,7 @@
       </c>
       <c r="I45" s="134" t="str">
         <f>_xll.qlFraRateHelper(H45,G45,B45,E45,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_43x55F#0003</v>
+        <v>EUR_YC1YRH_43x55F#0001</v>
       </c>
       <c r="J45" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I45)</f>
@@ -15348,7 +15346,7 @@
       </c>
       <c r="I46" s="134" t="str">
         <f>_xll.qlFraRateHelper(H46,G46,B46,E46,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_44x56F#0003</v>
+        <v>EUR_YC1YRH_44x56F#0001</v>
       </c>
       <c r="J46" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I46)</f>
@@ -15386,7 +15384,7 @@
       </c>
       <c r="I47" s="134" t="str">
         <f>_xll.qlFraRateHelper(H47,G47,B47,E47,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_45x57F#0003</v>
+        <v>EUR_YC1YRH_45x57F#0001</v>
       </c>
       <c r="J47" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I47)</f>
@@ -15424,7 +15422,7 @@
       </c>
       <c r="I48" s="134" t="str">
         <f>_xll.qlFraRateHelper(H48,G48,B48,E48,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_46x58F#0003</v>
+        <v>EUR_YC1YRH_46x58F#0001</v>
       </c>
       <c r="J48" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I48)</f>
@@ -15462,7 +15460,7 @@
       </c>
       <c r="I49" s="130" t="str">
         <f>_xll.qlFraRateHelper(H49,G49,B49,E49,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_47x59F#0003</v>
+        <v>EUR_YC1YRH_47x59F#0001</v>
       </c>
       <c r="J49" s="129" t="str">
         <f>_xll.ohRangeRetrieveError(I49)</f>
@@ -15528,7 +15526,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="186" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" s="162"/>
       <c r="C1" s="162"/>
@@ -15563,7 +15561,7 @@
       </c>
       <c r="L2" s="12" t="str">
         <f>Discounting</f>
-        <v>EurYC</v>
+        <v>EurON</v>
       </c>
       <c r="M2" s="107"/>
       <c r="N2" s="164"/>
@@ -15622,7 +15620,7 @@
       </c>
       <c r="L4" s="181" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC1YRH_AB12EBASIS_ibor1Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS_ibor1Y#0001</v>
       </c>
       <c r="M4" s="180" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -15686,7 +15684,7 @@
       </c>
       <c r="L6" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS1Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS1Y#0002</v>
       </c>
       <c r="M6" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -15739,7 +15737,7 @@
       </c>
       <c r="L7" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS15M#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS15M#0002</v>
       </c>
       <c r="M7" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -15788,7 +15786,7 @@
       </c>
       <c r="L8" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS18M#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS18M#0002</v>
       </c>
       <c r="M8" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -15837,7 +15835,7 @@
       </c>
       <c r="L9" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS21M#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS21M#0002</v>
       </c>
       <c r="M9" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -15886,7 +15884,7 @@
       </c>
       <c r="L10" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS2Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS2Y#0002</v>
       </c>
       <c r="M10" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -15944,7 +15942,7 @@
       </c>
       <c r="L11" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS3Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS3Y#0002</v>
       </c>
       <c r="M11" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -16002,7 +16000,7 @@
       </c>
       <c r="L12" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS4Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS4Y#0002</v>
       </c>
       <c r="M12" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -16060,7 +16058,7 @@
       </c>
       <c r="L13" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS5Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS5Y#0002</v>
       </c>
       <c r="M13" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -16118,7 +16116,7 @@
       </c>
       <c r="L14" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS6Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS6Y#0002</v>
       </c>
       <c r="M14" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -16176,7 +16174,7 @@
       </c>
       <c r="L15" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS7Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS7Y#0002</v>
       </c>
       <c r="M15" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -16228,7 +16226,7 @@
       </c>
       <c r="L16" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS8Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS8Y#0002</v>
       </c>
       <c r="M16" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -16277,7 +16275,7 @@
       </c>
       <c r="L17" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS9Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS9Y#0002</v>
       </c>
       <c r="M17" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -16326,7 +16324,7 @@
       </c>
       <c r="L18" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS10Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS10Y#0002</v>
       </c>
       <c r="M18" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -16375,7 +16373,7 @@
       </c>
       <c r="L19" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS11Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS11Y#0002</v>
       </c>
       <c r="M19" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -16424,7 +16422,7 @@
       </c>
       <c r="L20" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS12Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS12Y#0002</v>
       </c>
       <c r="M20" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -16473,7 +16471,7 @@
       </c>
       <c r="L21" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS13Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS13Y#0002</v>
       </c>
       <c r="M21" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -16522,7 +16520,7 @@
       </c>
       <c r="L22" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS14Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS14Y#0002</v>
       </c>
       <c r="M22" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -16571,7 +16569,7 @@
       </c>
       <c r="L23" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS15Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS15Y#0002</v>
       </c>
       <c r="M23" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -16620,7 +16618,7 @@
       </c>
       <c r="L24" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS16Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS16Y#0002</v>
       </c>
       <c r="M24" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -16669,7 +16667,7 @@
       </c>
       <c r="L25" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS17Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS17Y#0002</v>
       </c>
       <c r="M25" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -16718,7 +16716,7 @@
       </c>
       <c r="L26" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS18Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS18Y#0002</v>
       </c>
       <c r="M26" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -16767,7 +16765,7 @@
       </c>
       <c r="L27" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS19Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS19Y#0002</v>
       </c>
       <c r="M27" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -16816,7 +16814,7 @@
       </c>
       <c r="L28" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS20Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS20Y#0002</v>
       </c>
       <c r="M28" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -16865,7 +16863,7 @@
       </c>
       <c r="L29" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS21Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS21Y#0002</v>
       </c>
       <c r="M29" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -16914,7 +16912,7 @@
       </c>
       <c r="L30" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS22Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS22Y#0002</v>
       </c>
       <c r="M30" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -16963,7 +16961,7 @@
       </c>
       <c r="L31" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS23Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS23Y#0002</v>
       </c>
       <c r="M31" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -17012,7 +17010,7 @@
       </c>
       <c r="L32" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS24Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS24Y#0002</v>
       </c>
       <c r="M32" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -17061,7 +17059,7 @@
       </c>
       <c r="L33" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS25Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS25Y#0002</v>
       </c>
       <c r="M33" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -17110,7 +17108,7 @@
       </c>
       <c r="L34" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS26Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS26Y#0002</v>
       </c>
       <c r="M34" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -17159,7 +17157,7 @@
       </c>
       <c r="L35" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS27Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS27Y#0002</v>
       </c>
       <c r="M35" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -17208,7 +17206,7 @@
       </c>
       <c r="L36" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS28Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS28Y#0002</v>
       </c>
       <c r="M36" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -17257,7 +17255,7 @@
       </c>
       <c r="L37" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS29Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS29Y#0002</v>
       </c>
       <c r="M37" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -17306,7 +17304,7 @@
       </c>
       <c r="L38" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS30Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS30Y#0002</v>
       </c>
       <c r="M38" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -17355,7 +17353,7 @@
       </c>
       <c r="L39" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS35Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS35Y#0002</v>
       </c>
       <c r="M39" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -17404,7 +17402,7 @@
       </c>
       <c r="L40" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS40Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS40Y#0002</v>
       </c>
       <c r="M40" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -17453,7 +17451,7 @@
       </c>
       <c r="L41" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS50Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS50Y#0002</v>
       </c>
       <c r="M41" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -17502,7 +17500,7 @@
       </c>
       <c r="L42" s="166" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_AB12EBASIS60Y#0003</v>
+        <v>EUR_YC1YRH_AB12EBASIS60Y#0002</v>
       </c>
       <c r="M42" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>

</xml_diff>